<commit_message>
rerun distance models without bike share or transit access, run mode and carown models with both features
</commit_message>
<xml_diff>
--- a/outputs/ML_Results/dist_LR/Kassel.xlsx
+++ b/outputs/ML_Results/dist_LR/Kassel.xlsx
@@ -7,36 +7,36 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="summ49040422" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="summ49211876" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="summ49403896" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="summ49641176" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="summ49912485" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="summ50173247" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="summ50407456" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="summ50630545" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="summ50855219" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="summ51117779" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="summ51341804" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="summ51561859" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="summ51797192" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="summ52025819" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="summ52291884" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="summ52543423" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="summ52796610" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="summ53043030" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="summ53293859" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="summ53629142" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="summ53863738" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="summ54110346" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="summ54363474" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="summ54582939" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="summ54821000" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="summ55037635" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="summ55277683" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="summ55501771" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="summ55790783" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="summ56007279" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="summ25219841" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="summ25367751" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="summ25514181" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="summ25668715" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="summ25823978" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="summ25979184" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="summ26123109" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="summ26267340" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="summ26409742" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="summ26558126" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="summ26702151" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="summ26844244" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="summ26993701" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="summ27141364" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="summ27288744" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="summ27438760" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="summ27583024" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="summ27725738" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="summ27873788" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="summ28006245" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="summ28152110" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="summ28297379" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="summ28447896" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="summ28606894" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="summ28751608" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="summ28895984" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="summ29035804" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="summ29179363" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="summ29317716" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="summ29461529" sheetId="30" state="visible" r:id="rId30"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-21.7890317127104</v>
+        <v>-21.81734193764731</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -498,7 +498,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-206.4048348241577</v>
+        <v>-206.0827730538306</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>682.118328486466</v>
+        <v>683.0583216540253</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.447312672663648</v>
+        <v>2.44791355073087</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0003386694156733771</v>
+        <v>-0.0003384887910099633</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-172.6088770337043</v>
+        <v>-172.6771753894996</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -553,7 +553,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>162.1090976330887</v>
+        <v>162.1421030579131</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -564,7 +564,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-69.36247722463108</v>
+        <v>-69.47030205495869</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -575,42 +575,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-164.9893286986457</v>
+        <v>-165.1971631307934</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-26.29196636448591</v>
+        <v>14.74133236076779</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>14.7300265157734</v>
+        <v>-322.93444536453</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-322.758269140028</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -623,7 +612,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,7 +644,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24.14665155820192</v>
+        <v>23.70115246083577</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -666,7 +655,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-182.0131247901977</v>
+        <v>-173.6011182728789</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -677,7 +666,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>783.1759619224531</v>
+        <v>793.8471196040923</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -688,7 +677,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.5996523483980344</v>
+        <v>-0.5995076774159952</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -699,7 +688,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0003951465963869872</v>
+        <v>0.000396666303428093</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -710,7 +699,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>17.36000443266428</v>
+        <v>17.78324505158503</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -721,7 +710,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>173.9199617118598</v>
+        <v>173.9228800808887</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -732,7 +721,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-20.78080581464994</v>
+        <v>-20.55181934489861</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -743,42 +732,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>62.63613913215673</v>
+        <v>62.31735271378615</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-86.94065286073908</v>
+        <v>-11.13871842548218</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-11.18780541546017</v>
+        <v>-384.2282564242701</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-382.2385140921988</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -791,7 +769,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -823,7 +801,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>55.65166122071855</v>
+        <v>56.34635660564356</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -834,7 +812,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-498.1313793868737</v>
+        <v>-501.6952104758197</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -845,7 +823,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-289.3192155301417</v>
+        <v>-294.4161772797102</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -856,7 +834,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3231465600283094</v>
+        <v>-0.3236787410385153</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -867,7 +845,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.000433132839111307</v>
+        <v>-0.0004398692664352366</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -878,7 +856,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>30.76905818564859</v>
+        <v>30.3931022434387</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -889,7 +867,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>19.66134994301581</v>
+        <v>19.91243370901108</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -900,7 +878,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>65.95445724536427</v>
+        <v>66.82110960604319</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -911,42 +889,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>35.28167272604213</v>
+        <v>35.76529979824647</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>58.69306506012057</v>
+        <v>32.3416419130148</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>31.98489750150519</v>
+        <v>101.2914489737493</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>100.5223899109711</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -959,7 +926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -991,7 +958,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>184.6137891751601</v>
+        <v>184.5229446031801</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -1002,7 +969,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-27.88206350671771</v>
+        <v>-28.16304142020681</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -1013,7 +980,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1977.589350566545</v>
+        <v>1977.079418333249</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -1024,7 +991,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1917690387774791</v>
+        <v>0.1924538658922284</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -1035,7 +1002,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.000999651031121627</v>
+        <v>0.001000309088304344</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -1046,7 +1013,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>47.63578698278943</v>
+        <v>47.63864150496798</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -1057,7 +1024,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-34.32030534602282</v>
+        <v>-34.48319893157448</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -1068,7 +1035,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-874.3678120843688</v>
+        <v>-881.5829765027383</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -1079,42 +1046,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-267.4237559778498</v>
+        <v>-267.1770363185928</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>76.30854036542587</v>
+        <v>-217.4329429718844</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-214.4418944632789</v>
+        <v>-98.73607099436018</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-99.23484098754375</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1127,7 +1083,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1159,7 +1115,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27.25846530082326</v>
+        <v>27.29684524708202</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -1170,7 +1126,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-777.991538707327</v>
+        <v>-778.3015865912371</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -1181,7 +1137,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-549.9957488983086</v>
+        <v>-550.8532804316574</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -1192,7 +1148,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3448984437041469</v>
+        <v>-0.3447977598852319</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -1203,7 +1159,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.000132426500318598</v>
+        <v>0.0001323654360467279</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -1214,7 +1170,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-52.93536524249012</v>
+        <v>-52.96025701021931</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -1225,7 +1181,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>100.1310452211228</v>
+        <v>100.099341613833</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -1236,7 +1192,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20.86372884097338</v>
+        <v>20.89692202238015</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -1247,42 +1203,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-49.59326610244915</v>
+        <v>-49.60630224357365</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26.72525268539796</v>
+        <v>16.60456383078055</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>16.59526843016477</v>
+        <v>3.363446536483366</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>3.139451667660751</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1295,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1327,7 +1272,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>26.44732084882776</v>
+        <v>26.98247793032073</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -1338,7 +1283,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-115.0486463926296</v>
+        <v>-117.1734331710002</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -1349,7 +1294,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-200.2788002326693</v>
+        <v>-204.8728969809868</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -1360,7 +1305,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1596621796290343</v>
+        <v>-0.1606318026939406</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -1371,7 +1316,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0004923996397848186</v>
+        <v>-0.0004965301855515995</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -1382,7 +1327,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-51.69149178460742</v>
+        <v>-51.85715149895958</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -1393,7 +1338,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>19.5897848766613</v>
+        <v>19.80581996699318</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -1404,7 +1349,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31.62517954669721</v>
+        <v>32.27085961896745</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -1415,42 +1360,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>11.45101745115329</v>
+        <v>11.64675320765326</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>35.65897473554395</v>
+        <v>15.85796941559903</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>15.54580824004572</v>
+        <v>133.5004010067669</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>133.1056346819778</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1463,7 +1397,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1495,7 +1429,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>411.2691876290664</v>
+        <v>524.6613803768432</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -1506,7 +1440,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-634.887871590955</v>
+        <v>-726.0947175430847</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -1517,7 +1451,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-431.1023693986617</v>
+        <v>-539.8275389657611</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -1528,7 +1462,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.307872835743914</v>
+        <v>-0.3045789136899083</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -1539,7 +1473,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0004303892353963415</v>
+        <v>-0.0005000383937040936</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -1550,7 +1484,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>42.27495542581687</v>
+        <v>43.21012996449089</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -1561,7 +1495,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-14.83593448972226</v>
+        <v>-25.91030569491886</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -1572,7 +1506,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>159.2889458725904</v>
+        <v>240.8460211187157</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -1583,42 +1517,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>258.781625578662</v>
+        <v>336.9380991300159</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>445.9616276666566</v>
+        <v>180.4211731293199</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>131.3591260361545</v>
+        <v>225.2426923278736</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>183.8918552026221</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1631,7 +1554,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1663,7 +1586,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>610.9622438974257</v>
+        <v>614.3616332983897</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -1674,7 +1597,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-2187.895770676633</v>
+        <v>-2200.456437145802</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -1685,7 +1608,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>296.5515493766002</v>
+        <v>294.5463255931509</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -1696,7 +1619,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3314833534697248</v>
+        <v>-0.3310386705190682</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -1707,7 +1630,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.001189748934601058</v>
+        <v>-0.001196636884181619</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -1718,7 +1641,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>171.1644226291307</v>
+        <v>172.0586699685102</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -1729,7 +1652,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-2.351056149595777</v>
+        <v>-2.41976842404307</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -1740,7 +1663,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>465.2822463818115</v>
+        <v>468.1342292642212</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -1751,42 +1674,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>490.8470119267922</v>
+        <v>493.5924496898674</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>179.5265263617787</v>
+        <v>236.491687655481</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>235.1528909359231</v>
+        <v>143.0312428829073</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>142.1626056184564</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1799,7 +1711,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1831,7 +1743,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>117.3035546965289</v>
+        <v>117.3286552210424</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -1842,7 +1754,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>965.309337841109</v>
+        <v>965.6495881512462</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -1853,7 +1765,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>996.4209298394021</v>
+        <v>996.1069785449722</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -1864,7 +1776,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3813230586707302</v>
+        <v>-0.381444963959321</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -1875,7 +1787,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0002972650752156494</v>
+        <v>0.0002970902270562142</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -1886,7 +1798,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18.09410258117148</v>
+        <v>18.08730718528494</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -1897,7 +1809,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>116.352375879814</v>
+        <v>116.3842975530408</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -1908,7 +1820,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-250.0882955024553</v>
+        <v>-250.1073400706177</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -1919,42 +1831,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-130.5226345033171</v>
+        <v>-130.5285002399596</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>6.429145058104979</v>
+        <v>-32.96025943634013</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-32.95379211211549</v>
+        <v>-341.3826186107931</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-341.3432519626957</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1967,7 +1868,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1999,7 +1900,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>590.8375151513551</v>
+        <v>591.489376539862</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -2010,7 +1911,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-403.6793046495584</v>
+        <v>-408.8787178120415</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -2021,7 +1922,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-434.7699357633724</v>
+        <v>-442.4234671560355</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -2032,7 +1933,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.05788917431543961</v>
+        <v>0.06015698213713727</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -2043,7 +1944,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0001757389934520195</v>
+        <v>-0.0001867730113768023</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -2054,7 +1955,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>52.11277198439907</v>
+        <v>51.44481140544957</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -2065,7 +1966,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-2.298785630066021</v>
+        <v>-1.858754746781244</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -2076,7 +1977,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-408.7543053078833</v>
+        <v>-408.7556287097043</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -2087,42 +1988,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-5844.223793674018</v>
+        <v>-5845.786653811092</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>124.5527209356102</v>
+        <v>1246.732851701281</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1246.344805326402</v>
+        <v>121.5940336082265</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>120.6010184914418</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2135,7 +2025,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2167,7 +2057,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>77.18337266459412</v>
+        <v>78.21494588798646</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -2178,7 +2068,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-535.113128861838</v>
+        <v>-542.1663166183062</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -2189,7 +2079,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-242.7010661476185</v>
+        <v>-246.5776053126656</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -2200,7 +2090,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3140761471117171</v>
+        <v>-0.3145339620247376</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -2211,7 +2101,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0004204103755269259</v>
+        <v>-0.0004281228336417498</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -2222,7 +2112,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>37.99994263211602</v>
+        <v>37.99324410739075</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -2233,7 +2123,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>17.28336099442063</v>
+        <v>17.46314518205061</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -2244,7 +2134,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>113.0286424639091</v>
+        <v>114.5072123673499</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -2255,42 +2145,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>54.45213858375303</v>
+        <v>55.17407200596074</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>71.5812221557087</v>
+        <v>54.8311934231557</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>54.13633118480971</v>
+        <v>98.30810051129356</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>97.46414183362083</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2303,7 +2182,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2335,7 +2214,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.748626200132561</v>
+        <v>0.7482828360712581</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -2346,7 +2225,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-446.627664583048</v>
+        <v>-446.6245786097563</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -2357,7 +2236,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>199.4652818525044</v>
+        <v>199.4724450299895</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -2368,7 +2247,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.06398652529778148</v>
+        <v>-0.0639863340812028</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -2379,7 +2258,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0003714731577884211</v>
+        <v>-0.0003714667935958556</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -2390,7 +2269,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.832862000849531</v>
+        <v>9.833097338733367</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -2401,7 +2280,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.09467017900723107</v>
+        <v>-0.0950413298576791</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -2412,7 +2291,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-10.77307112796572</v>
+        <v>-10.77311320121964</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -2423,42 +2302,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-5.82499808256901</v>
+        <v>-5.825080811519218</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.06946898831149895</v>
+        <v>3.238365896867887</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.238372982291708</v>
+        <v>112.4840613926978</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>112.4844943639022</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2471,7 +2339,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2503,7 +2371,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-12.81196635013126</v>
+        <v>-12.81215364069987</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -2514,7 +2382,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-735.6341429422287</v>
+        <v>-735.6349346102841</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -2525,7 +2393,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-479.1816027977173</v>
+        <v>-479.2366244390412</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -2536,7 +2404,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.2332441382040422</v>
+        <v>-0.233056925241842</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -2547,7 +2415,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9.061297960450342e-05</v>
+        <v>9.052796100161799e-05</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -2558,7 +2426,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-48.78794602716188</v>
+        <v>-48.78741905617422</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -2569,7 +2437,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>102.0811326419762</v>
+        <v>102.0805426409323</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -2580,7 +2448,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>33.62899909073957</v>
+        <v>33.63223845383386</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -2591,42 +2459,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-132.9958487017978</v>
+        <v>-133.0016948725318</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5.268901767593368</v>
+        <v>31.8565412039305</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>31.85513839731446</v>
+        <v>-19.70549816464205</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-19.70722181291703</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2639,7 +2496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2671,7 +2528,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>366.9178375123483</v>
+        <v>377.5827178329528</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -2682,7 +2539,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>558.5056043862389</v>
+        <v>569.23248289465</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -2693,7 +2550,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>768.4756260653979</v>
+        <v>737.2751179694818</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -2704,7 +2561,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.2978178300815824</v>
+        <v>-0.3038589377909611</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -2715,7 +2572,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0003684236159856536</v>
+        <v>0.0003580423686831587</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -2726,7 +2583,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7.97304678012982</v>
+        <v>7.114558237352952</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -2737,7 +2594,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>100.6398984836752</v>
+        <v>102.4390951093933</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -2748,7 +2605,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-2472.564188022232</v>
+        <v>-2552.444266446253</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -2759,42 +2616,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-410.6430640265612</v>
+        <v>-420.9666803780965</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>458.1549198882099</v>
+        <v>-827.6713719319441</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-800.1062800978889</v>
+        <v>-259.2893013625956</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-259.2838018331133</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2807,7 +2653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2839,7 +2685,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>25.46053555074509</v>
+        <v>25.72627711136887</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -2850,7 +2696,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-904.2337062589213</v>
+        <v>-906.3343274540573</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -2861,7 +2707,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-48.76985370906178</v>
+        <v>-53.60015738341116</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -2872,7 +2718,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.0704907885169318</v>
+        <v>-0.07059571980761647</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -2883,7 +2729,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.001071622764609424</v>
+        <v>-0.001075932586153339</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -2894,7 +2740,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-27.47122317135211</v>
+        <v>-27.63106961305773</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -2905,7 +2751,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>138.2116375621156</v>
+        <v>138.4694190860382</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -2916,7 +2762,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-20.13431815063461</v>
+        <v>-20.13182673899406</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -2927,42 +2773,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-87.8182616487006</v>
+        <v>-88.120114315389</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>46.62091636316418</v>
+        <v>21.75007139195538</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>21.66935818247673</v>
+        <v>-132.7837919647532</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-133.0581710376057</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2975,7 +2810,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3007,7 +2842,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>414.1932929165787</v>
+        <v>671.7751006212729</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -3018,7 +2853,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>126.0117038428184</v>
+        <v>217.3291138219356</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -3029,7 +2864,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-271.8967929141677</v>
+        <v>-316.0821665204624</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -3040,7 +2875,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.09805012009307634</v>
+        <v>-0.05745653433854025</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -3051,7 +2886,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-3.289837571361729e-06</v>
+        <v>4.052628246347615e-05</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -3062,7 +2897,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-22.74559823174525</v>
+        <v>-38.2620473674944</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -3073,7 +2908,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30.53557333942688</v>
+        <v>35.15585753991701</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -3084,7 +2919,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-599.1018560245539</v>
+        <v>-985.0170311234942</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -3095,42 +2930,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>160.0185742291492</v>
+        <v>257.8134784840408</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>624.3271977701843</v>
+        <v>-229.6458982704207</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-140.2854802568982</v>
+        <v>19.788722672836</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>30.00673462969792</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3143,7 +2967,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3175,7 +2999,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>956.8725645801742</v>
+        <v>976.4817644185591</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -3186,7 +3010,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>470.3673111368546</v>
+        <v>469.6054705913087</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -3197,7 +3021,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1058.557930678718</v>
+        <v>1056.853166275785</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -3208,7 +3032,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1360647026359684</v>
+        <v>-0.1334659995265044</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -3219,7 +3043,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0001539523057746497</v>
+        <v>0.0001500593323713708</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -3230,7 +3054,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.354004376738501</v>
+        <v>4.096818717188583</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -3241,7 +3065,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>121.0388147460414</v>
+        <v>121.3246349736256</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -3252,7 +3076,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>627.45473727641</v>
+        <v>642.6226423589806</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -3263,42 +3087,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1326.040101938115</v>
+        <v>1358.229176339487</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>264.1806509199487</v>
+        <v>203.6580973906927</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>200.0971982782326</v>
+        <v>-363.5553419050393</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-362.8838428915844</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3311,7 +3124,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3343,7 +3156,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>36.19542526901304</v>
+        <v>36.39272702719106</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -3354,7 +3167,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>430.373623321816</v>
+        <v>434.1791382082902</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -3365,7 +3178,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>897.0440031860103</v>
+        <v>900.4929658024848</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -3376,7 +3189,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.0545696473907733</v>
+        <v>0.0470581517641504</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -3387,7 +3200,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0001787499670885878</v>
+        <v>0.0001832566408418164</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -3398,7 +3211,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>11.42885502087965</v>
+        <v>11.53033998187919</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -3409,7 +3222,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>104.9354011170871</v>
+        <v>104.720607799737</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -3420,7 +3233,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-47.4394614216427</v>
+        <v>-47.59832089093342</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -3431,42 +3244,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-54.8464103305007</v>
+        <v>-54.90047219570067</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-68.25765900407117</v>
+        <v>9.823581864558696</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.813744335721296</v>
+        <v>-296.3583138518492</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-296.5906736058162</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3479,7 +3281,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3511,7 +3313,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-50.03994587558098</v>
+        <v>-50.35305540048191</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -3522,7 +3324,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-359.0013462618845</v>
+        <v>-349.172779148465</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -3533,7 +3335,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>733.7142378559749</v>
+        <v>735.0225215877881</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -3544,7 +3346,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5557502012640443</v>
+        <v>0.5461504056139361</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -3555,7 +3357,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.746550230156317e-05</v>
+        <v>5.674487369773337e-05</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -3566,7 +3368,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-14.16792750578918</v>
+        <v>-12.07800492060667</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -3577,7 +3379,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-35.69162143645306</v>
+        <v>-36.16881154887236</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -3588,7 +3390,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1315.21753093583</v>
+        <v>-1318.199165935745</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -3599,42 +3401,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-4995.650551090061</v>
+        <v>-5007.601673699892</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-247.8104135723996</v>
+        <v>543.9253849116124</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>542.6854688397784</v>
+        <v>148.9378720378156</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>151.0728494322559</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3647,7 +3438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3679,7 +3470,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5489.169105911159</v>
+        <v>5953.054321970962</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -3690,7 +3481,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-545.5582720391048</v>
+        <v>-559.0821135226897</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -3701,7 +3492,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-6.980930120974563</v>
+        <v>-58.05483814477475</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -3712,7 +3503,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.4500266946611871</v>
+        <v>-0.454770382540044</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -3723,7 +3514,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0006183420269952377</v>
+        <v>-0.0006542231754682886</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -3734,7 +3525,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-21.15350824704092</v>
+        <v>-26.7095261300276</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -3745,7 +3536,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6.824131380059782</v>
+        <v>6.766655383563887</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -3756,7 +3547,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1978.892291786522</v>
+        <v>-2154.913709963624</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -3767,42 +3558,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3963.605470314287</v>
+        <v>4297.871431481164</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2060.306502717628</v>
+        <v>-467.0839332802187</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-426.4552961024399</v>
+        <v>48.84917936309375</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>46.37576051174517</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3815,7 +3595,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3847,7 +3627,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>64.44977420748432</v>
+        <v>64.7539327181437</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -3858,7 +3638,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>195.6746654872089</v>
+        <v>199.2094892754145</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -3869,7 +3649,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1905.737465289434</v>
+        <v>1913.578360461334</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -3880,7 +3660,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.7255509371546562</v>
+        <v>0.7246419078135968</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -3891,7 +3671,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.001130801493946115</v>
+        <v>0.001134166202928489</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -3902,7 +3682,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>52.44196620690334</v>
+        <v>52.37877059309731</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -3913,7 +3693,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-120.4076380803685</v>
+        <v>-120.5079662564764</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -3924,7 +3704,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-451.4605490587309</v>
+        <v>-453.4871304542506</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -3935,42 +3715,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-4636.880246132886</v>
+        <v>-4657.474624969869</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-339.4742812135244</v>
+        <v>863.7451735236609</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>859.9620458666941</v>
+        <v>97.62752506726278</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>98.45913658934094</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3983,7 +3752,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4015,7 +3784,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-17.07847036405119</v>
+        <v>-17.59539777607804</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -4026,7 +3795,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>156.9658545824061</v>
+        <v>162.3012588124866</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -4037,7 +3806,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>566.3698587347699</v>
+        <v>582.2234806474826</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -4048,7 +3817,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.2830309064852323</v>
+        <v>-0.2872821808126027</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -4059,7 +3828,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0001853402906330202</v>
+        <v>-0.0001754250348720977</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -4070,7 +3839,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-1.158697679131535</v>
+        <v>-0.3862875091022033</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -4081,7 +3850,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>126.9909693249581</v>
+        <v>127.6559415805547</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -4092,7 +3861,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9.072521793499106</v>
+        <v>9.281627755387362</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -4103,42 +3872,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>6.748115312175287</v>
+        <v>6.854183503504657</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-104.7651352283456</v>
+        <v>-1.73998391367204</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-1.715711304383591</v>
+        <v>-260.2400811936229</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-256.084384087078</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4151,7 +3909,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4183,7 +3941,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-157.1841039875746</v>
+        <v>-179.747841385114</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -4194,7 +3952,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>667.5007971924144</v>
+        <v>656.530539119442</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -4205,7 +3963,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>482.6747811059204</v>
+        <v>558.4349441522791</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -4216,7 +3974,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.1059780750729145</v>
+        <v>-0.1454419166115879</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -4227,7 +3985,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0002929344655427809</v>
+        <v>0.0003112168996307612</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -4238,7 +3996,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-20.48318205690055</v>
+        <v>-16.07818064553305</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -4249,7 +4007,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>44.74030280369846</v>
+        <v>56.26776802094673</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -4260,7 +4018,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1288.335266092543</v>
+        <v>-1409.699154071597</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -4271,42 +4029,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>359.0189652198565</v>
+        <v>396.8917421493456</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-503.7671656065932</v>
+        <v>-764.7301108418769</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-696.4746745917309</v>
+        <v>-121.4064719915123</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-85.4655368906765</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4319,7 +4066,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4351,7 +4098,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-71.24413363648455</v>
+        <v>-262.7515885688047</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -4362,7 +4109,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-144.3064881450637</v>
+        <v>38.06000162257897</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -4373,7 +4120,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25.89806839039301</v>
+        <v>683.1848739829684</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -4384,7 +4131,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.08451559514309973</v>
+        <v>-0.1806461960936776</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -4395,7 +4142,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0005822124588976008</v>
+        <v>-0.0009652177790229217</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -4406,7 +4153,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>51.31474230769835</v>
+        <v>87.85926643295431</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -4417,7 +4164,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-160.412364810132</v>
+        <v>-226.441859391271</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -4428,7 +4175,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3039.748491075079</v>
+        <v>9879.459884236625</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -4439,42 +4186,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1282.164146465695</v>
+        <v>4155.719861276579</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-4985.085709341482</v>
+        <v>1241.846264320959</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>383.3899287646018</v>
+        <v>552.4618363293305</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>491.9548225077248</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4487,7 +4223,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4519,7 +4255,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>636.0795005426894</v>
+        <v>733.5585862742455</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -4530,7 +4266,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2686.615864304036</v>
+        <v>3498.579250052331</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -4541,7 +4277,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-2833.344955840766</v>
+        <v>-3167.384394526434</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -4552,7 +4288,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3831909421303961</v>
+        <v>-0.3744073861591064</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -4563,7 +4299,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.001127094678557059</v>
+        <v>-0.001007468743754213</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -4574,7 +4310,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-504.6352788702393</v>
+        <v>-602.6237868932244</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -4585,7 +4321,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>163.2843624043013</v>
+        <v>183.616403042637</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -4596,7 +4332,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>973.3766360493028</v>
+        <v>1134.319423371678</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -4607,42 +4343,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1062.501622714773</v>
+        <v>1264.722900059627</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-1900.521059371957</v>
+        <v>-34.390687316975</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-11.02540776929831</v>
+        <v>167.3433393487597</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>180.8936808862313</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4655,7 +4380,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4687,7 +4412,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>74.84843773880606</v>
+        <v>74.80224731458949</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -4698,7 +4423,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>714.7048033700817</v>
+        <v>713.8333752195206</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -4709,7 +4434,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>870.0704900860123</v>
+        <v>871.5859261966075</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -4720,7 +4445,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.3519508886079428</v>
+        <v>-0.3515221542328236</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -4731,7 +4456,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0003106807221000287</v>
+        <v>0.0003113527893961717</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -4742,7 +4467,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>11.27492163077875</v>
+        <v>11.31569061026838</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -4753,7 +4478,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>107.346447708465</v>
+        <v>107.236022314589</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -4764,7 +4489,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-77.11841498887907</v>
+        <v>-77.15350582227524</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -4775,42 +4500,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-89.46552085158069</v>
+        <v>-89.49130998875998</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-25.87555162017975</v>
+        <v>16.0440175173454</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>16.03691363220334</v>
+        <v>-290.0036970748909</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-290.0604229102524</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4823,7 +4537,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4855,7 +4569,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-35.03099055076144</v>
+        <v>-35.32600366570853</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -4866,7 +4580,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-363.924288663327</v>
+        <v>-361.1754634096357</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -4877,7 +4591,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-422.5319315529567</v>
+        <v>-415.7798820710941</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -4888,7 +4602,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.04868575030827599</v>
+        <v>-0.04789678322038693</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -4899,7 +4613,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9.947129704554296e-05</v>
+        <v>0.0001020504570515803</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -4910,7 +4624,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>59.3874512454541</v>
+        <v>59.19587287541555</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -4921,7 +4635,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.263422482025646</v>
+        <v>5.26785129202095</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -4932,7 +4646,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1268.558056963911</v>
+        <v>-1271.945466112494</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -4943,42 +4657,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-5165.353240560626</v>
+        <v>-5177.18138833483</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-249.3059050386736</v>
+        <v>576.5889221393656</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>575.3766929830674</v>
+        <v>98.17000625535528</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>99.01233048404987</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4991,7 +4694,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5023,7 +4726,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2233.403744315921</v>
+        <v>3081.604591662888</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -5034,7 +4737,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1094.709230108992</v>
+        <v>-1439.463326296258</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -5045,7 +4748,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>170.4042914594788</v>
+        <v>-40.88019494310583</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -5056,7 +4759,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.03271459521415832</v>
+        <v>-0.09787830950397325</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -5067,7 +4770,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.000305634046504692</v>
+        <v>-0.0005184117311221609</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -5078,7 +4781,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>38.09729963176392</v>
+        <v>45.5563352732205</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -5089,7 +4792,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-145.2697530780722</v>
+        <v>-165.5298061423973</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -5100,7 +4803,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-1534.658515043393</v>
+        <v>-2144.149299508473</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -5111,42 +4814,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1296.918725873049</v>
+        <v>1783.500138572959</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1967.705252385924</v>
+        <v>-380.7374164125259</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-265.495423180618</v>
+        <v>518.8807457909147</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>436.816596299537</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5159,7 +4851,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5191,7 +4883,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-6.095694768707602</v>
+        <v>-6.096353837705214</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -5202,7 +4894,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-293.1847290205634</v>
+        <v>-293.2393441554311</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -5213,7 +4905,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.085414036580914</v>
+        <v>5.964719273028322</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -5224,7 +4916,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.6636945312223652</v>
+        <v>-0.6636790933301617</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -5235,7 +4927,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.0005125064232096681</v>
+        <v>0.0005124264054809594</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -5246,7 +4938,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>116.6500464787662</v>
+        <v>116.6476823243863</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -5257,7 +4949,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>69.69114341690539</v>
+        <v>69.69126453477151</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -5268,7 +4960,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-27.87267907003859</v>
+        <v>-27.88486726041488</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -5279,42 +4971,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-17.28722092088606</v>
+        <v>-17.28335195692467</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3.375781852500907</v>
+        <v>-7.90991634749038</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-7.901864099986952</v>
+        <v>-184.6225209857965</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-184.643940993009</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5327,7 +5008,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5359,7 +5040,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2660.713663002718</v>
+        <v>18898.79084215172</v>
       </c>
       <c r="C2" t="inlineStr"/>
     </row>
@@ -5370,7 +5051,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-697.4243685174961</v>
+        <v>-453.3088169412958</v>
       </c>
       <c r="C3" t="inlineStr"/>
     </row>
@@ -5381,7 +5062,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-334.956669696785</v>
+        <v>1380.665404158863</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
@@ -5392,7 +5073,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2330751076662132</v>
+        <v>0.2073803679972452</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
@@ -5403,7 +5084,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.0002478579547514422</v>
+        <v>-0.001005600806963575</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
@@ -5414,7 +5095,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-37.20365798599133</v>
+        <v>25.0997117754867</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
@@ -5425,7 +5106,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>61.90674209331345</v>
+        <v>-173.0504909664398</v>
       </c>
       <c r="C8" t="inlineStr"/>
     </row>
@@ -5436,7 +5117,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3694.177791461819</v>
+        <v>25873.73855000188</v>
       </c>
       <c r="C9" t="inlineStr"/>
     </row>
@@ -5447,42 +5128,31 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-497.2942611563287</v>
+        <v>-2620.297351617261</v>
       </c>
       <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>bike_lane_share_res</t>
+          <t>Commute_Trip</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-11366.14191759953</v>
+        <v>5473.349384502306</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Commute_Trip</t>
+          <t>Age</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>804.2606156776334</v>
+        <v>-8.976635418879027</v>
       </c>
       <c r="C12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>-14.47025718378927</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>